<commit_message>
changed study docs location
</commit_message>
<xml_diff>
--- a/data/study/questionaire.xlsx
+++ b/data/study/questionaire.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terfu\Desktop\2021-fastReach\data\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D02E86-E29C-43C2-81B6-681DB7570B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2330CC40-FAB3-4B0B-AD28-D9301CF16B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2760" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="input" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="3" r:id="rId1"/>
+    <sheet name="data_old" sheetId="1" r:id="rId2"/>
+    <sheet name="input" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>pID</t>
   </si>
@@ -40,9 +41,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>first_block</t>
-  </si>
-  <si>
     <t>control_random</t>
   </si>
   <si>
@@ -116,6 +114,60 @@
   </si>
   <si>
     <t>pilot cindy</t>
+  </si>
+  <si>
+    <t>anisha</t>
+  </si>
+  <si>
+    <t>first_language</t>
+  </si>
+  <si>
+    <t>englisch</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>first_block_old</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>item_baseline</t>
+  </si>
+  <si>
+    <t>text_baseline</t>
+  </si>
+  <si>
+    <t>item_passive</t>
+  </si>
+  <si>
+    <t>text_passive</t>
+  </si>
+  <si>
+    <t>item_agency</t>
+  </si>
+  <si>
+    <t>text_agency</t>
+  </si>
+  <si>
+    <t>cap_size</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>interview_trans</t>
+  </si>
+  <si>
+    <t>I chose to press the screen; I was using my free will</t>
+  </si>
+  <si>
+    <t>I had not choice; it wans't me</t>
+  </si>
+  <si>
+    <t>it happend sometimes, but sometimes not; I felt pretty much in controll;</t>
   </si>
 </sst>
 </file>
@@ -278,7 +330,348 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="40">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -598,24 +991,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{898ACBF7-4D21-4B0A-9A89-8EAC5D324AC9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O43" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O43" xr:uid="{898ACBF7-4D21-4B0A-9A89-8EAC5D324AC9}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{7E5B5C79-7639-49FF-A5C0-B637BA4C0D8E}" name="pID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{41AECC35-EB26-4397-9149-6F3197B5A029}" name="comments" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{B3A0E20F-7B2E-4689-8012-78D7097C0A99}" name="vaild" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{B972C5BD-835D-4517-9CE0-90D97620E0C7}" name="age" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{E2253D4D-3D7F-4048-9352-DC85256E7A51}" name="sex" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{0DE115FF-04B2-4897-90EF-E795A7BBC6E7}" name="gender" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{F5769B9E-983D-4F9F-9B29-7F787CE76F6F}" name="first_block" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{DE468D1F-28AD-44E2-96E0-083039BB2F4F}" name="control_agency" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{72040056-0B2C-46D2-9ECF-5308D0277E72}" name="control_random" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{E8085B4E-D2B7-4C9E-963F-7E35A912A3ED}" name="time_expectation" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{DE959692-669E-4278-B42B-32B082371A92}" name="embodiment" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{59481544-AC36-40FD-A2D4-0261433D07E3}" name="interview_agency" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C3FD13EB-427E-4C1C-9D1B-D98BCB847AA1}" name="interview_agency_trans" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{A69CD8B8-0723-4AB4-B280-9B54255EB8AF}" name="interview_random" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{167DE025-67DC-4AED-96D2-356E1D1322BC}" name="interview_random_trans" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3781E842-391C-4515-9220-623679F29724}" name="Tabelle13" displayName="Tabelle13" ref="A1:P40" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:P40" xr:uid="{3781E842-391C-4515-9220-623679F29724}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{FCC9522A-6C94-43D7-83B4-03F95C940CDD}" name="pID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C390E5F0-49A4-4049-8E63-977FF8DD5583}" name="comments" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{7DE46A29-514D-4795-8A70-53BB141B9BD3}" name="vaild" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{4F80C496-9083-4346-857D-6273DDF84127}" name="cap_size" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A98F4A19-62CE-4A68-9E0B-9B9412578D3B}" name="age" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{B285662B-70D7-4412-9634-C655D2F6FAAF}" name="first_language" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{D3079AF4-78C4-4424-BC52-D4BACE441CEF}" name="sex" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{13D4C27F-003A-4155-826E-39CB9D4765A6}" name="gender" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E51D2886-8623-4285-921B-205320B896AD}" name="item_baseline" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{FC411175-3DAA-407B-B025-10B0A0590C09}" name="text_baseline" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{72220960-232B-47EB-B2BB-CC5C3ED2C9E4}" name="item_passive" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{D97EE890-F9BD-4FDD-8ACF-33E745753FD9}" name="text_passive" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{27618442-AA2C-4E3B-AA9F-E5D93301C788}" name="item_agency" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{6353A30F-0F0F-43FC-84B7-22CDEAF8D9A8}" name="text_agency" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{C93F8F74-28FE-457C-9F3D-537FED0ABB5B}" name="interview" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{897D179D-0D5A-4D7C-B1EC-7F9F27BB046A}" name="interview_trans" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{898ACBF7-4D21-4B0A-9A89-8EAC5D324AC9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P43" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="A1:P43" xr:uid="{898ACBF7-4D21-4B0A-9A89-8EAC5D324AC9}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{7E5B5C79-7639-49FF-A5C0-B637BA4C0D8E}" name="pID" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{41AECC35-EB26-4397-9149-6F3197B5A029}" name="comments" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{B3A0E20F-7B2E-4689-8012-78D7097C0A99}" name="vaild" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B972C5BD-835D-4517-9CE0-90D97620E0C7}" name="age" dataDxfId="32"/>
+    <tableColumn id="16" xr3:uid="{4DEC96F3-E8F3-4783-ABFE-497A2FF85D5D}" name="first_language" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E2253D4D-3D7F-4048-9352-DC85256E7A51}" name="sex" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{0DE115FF-04B2-4897-90EF-E795A7BBC6E7}" name="gender" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{F5769B9E-983D-4F9F-9B29-7F787CE76F6F}" name="first_block_old" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{DE468D1F-28AD-44E2-96E0-083039BB2F4F}" name="control_agency" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{72040056-0B2C-46D2-9ECF-5308D0277E72}" name="control_random" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{E8085B4E-D2B7-4C9E-963F-7E35A912A3ED}" name="time_expectation" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{DE959692-669E-4278-B42B-32B082371A92}" name="embodiment" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{59481544-AC36-40FD-A2D4-0261433D07E3}" name="interview_agency" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{C3FD13EB-427E-4C1C-9D1B-D98BCB847AA1}" name="interview_agency_trans" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{A69CD8B8-0723-4AB4-B280-9B54255EB8AF}" name="interview_random" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{167DE025-67DC-4AED-96D2-356E1D1322BC}" name="interview_random_trans" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -883,183 +1302,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B57C1C4-90EB-4FAA-B01F-C85005A263D9}">
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="13" width="22.7109375" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="25" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="14" width="22.7109375" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>3</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1067,9 +1454,10 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1084,9 +1472,10 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="1"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1101,9 +1490,10 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="1"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1118,9 +1508,10 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1135,9 +1526,10 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="1"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1152,9 +1544,10 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="1"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1169,9 +1562,10 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="1"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1186,9 +1580,10 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="1"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1203,9 +1598,10 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="1"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1220,9 +1616,10 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="1"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1237,9 +1634,10 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="1"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1254,9 +1652,10 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="1"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1271,9 +1670,10 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1288,9 +1688,10 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="1"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1305,9 +1706,10 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1322,9 +1724,10 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="1"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1339,9 +1742,10 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="1"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1356,9 +1760,10 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1373,9 +1778,10 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O22" s="1"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1390,9 +1796,10 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O23" s="1"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1407,9 +1814,10 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="1"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1424,9 +1832,10 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="1"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1441,9 +1850,10 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O26" s="1"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1458,9 +1868,10 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="1"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1475,9 +1886,10 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O28" s="1"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1492,9 +1904,10 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
-      <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="1"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1509,9 +1922,10 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="1"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1526,9 +1940,10 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="1"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1543,9 +1958,10 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O32" s="1"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1560,9 +1976,10 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="2"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="1"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1577,9 +1994,10 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
-      <c r="O34" s="2"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="1"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1594,9 +2012,10 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
-      <c r="O35" s="2"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="1"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1611,9 +2030,10 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
-      <c r="O36" s="2"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="1"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1628,9 +2048,10 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="2"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="1"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1645,9 +2066,10 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="2"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="1"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1662,9 +2084,901 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="1"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87374DDD-D98E-45CD-82ED-836952EBD639}">
+          <x14:formula1>
+            <xm:f>input!$F$1:$F$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F064084-E5CA-43F6-84C9-D832712E978F}">
+          <x14:formula1>
+            <xm:f>input!$B$1:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4:K40 K2 I2:I40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4F7E524-9787-4753-B7B6-948DE97645E8}">
+          <x14:formula1>
+            <xm:f>input!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:H40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2CCC0AF0-F234-472B-9419-6B5CE4C1E9CE}">
+          <x14:formula1>
+            <xm:f>input!$B$1:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M40</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="14" width="22.7109375" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1679,9 +2993,10 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
-      <c r="O40" s="2"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="1"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1696,9 +3011,10 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="2"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="1"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1713,9 +3029,10 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="2"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="1"/>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1723,14 +3040,15 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="5"/>
+      <c r="H43" s="1"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="1"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
-      <c r="O43" s="6"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1745,37 +3063,37 @@
           <x14:formula1>
             <xm:f>input!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:F43</xm:sqref>
+          <xm:sqref>F2:G43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{173B9FC7-D1C0-4BC9-B942-141EAAC7E903}">
           <x14:formula1>
             <xm:f>input!$B$1:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:I43 J2:O2</xm:sqref>
+          <xm:sqref>I2:J43 K2:P2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6E10E36-6146-42BE-AC2A-326405C48E3F}">
           <x14:formula1>
             <xm:f>input!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>J43</xm:sqref>
+          <xm:sqref>K43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE5486A-38C5-42C4-A79B-67E2B27CF71D}">
           <x14:formula1>
             <xm:f>input!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K43</xm:sqref>
+          <xm:sqref>L3:L43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9F34237-43DB-4126-957F-DA8F1BF51574}">
           <x14:formula1>
             <xm:f>input!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G43</xm:sqref>
+          <xm:sqref>H2:H43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3FF9800E-F082-428B-A6BE-C4F1FC00F1A2}">
           <x14:formula1>
             <xm:f>input!$D$1:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J42</xm:sqref>
+          <xm:sqref>K3:K42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4EF5CB3-2B90-4A22-9B97-879F27115F59}">
           <x14:formula1>
@@ -1789,99 +3107,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6637884F-B4B6-4228-B291-1A8F389D8877}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>-3</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>-2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>-1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>